<commit_message>
released dustbike core to fab
</commit_message>
<xml_diff>
--- a/core_hardware/Dustbike_Core/Project Outputs for Dustbike_Core/Dustbike_Core.xlsx
+++ b/core_hardware/Dustbike_Core/Project Outputs for Dustbike_Core/Dustbike_Core.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TomByrne\dustbike19\core_hardware\Dustbike_Core\Project Outputs for Dustbike_Core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F9E0336-90A3-4421-BF08-E6DAEAE1843F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{430D6823-AFD6-4644-BB29-8E5836BCEF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5940" windowWidth="38700" windowHeight="15060" xr2:uid="{38123167-F1D5-45A1-9262-C03F8D4940F6}"/>
+    <workbookView xWindow="0" yWindow="5940" windowWidth="38700" windowHeight="15060" xr2:uid="{5521C8D5-FE09-4C87-9169-7BDF32D752A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Dustbike_Core" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
   <si>
     <t>Description</t>
   </si>
@@ -54,43 +54,49 @@
     <t>Manufacturer Part Number 1</t>
   </si>
   <si>
-    <t>Supplier 1</t>
-  </si>
-  <si>
-    <t>Supplier Part Number 1</t>
-  </si>
-  <si>
-    <t>CAP CER 1000PF 50V X7R 0603, CAP CER 0.1UF 25V X5R 0603</t>
-  </si>
-  <si>
-    <t>C1, C4</t>
+    <t>CAP CER 1000PF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>C1</t>
   </si>
   <si>
     <t>Samsung Electro-Mechanics</t>
   </si>
   <si>
-    <t>CL10B102KB8NNNC, CL10A104KA8NNNC</t>
-  </si>
-  <si>
-    <t>Digi-Key</t>
-  </si>
-  <si>
-    <t>1276-1018-1-ND, 1276-1857-1-ND</t>
-  </si>
-  <si>
-    <t>CAP ALUM 47UF 20% 25V RADIAL, CAP ALUM 10UF 20% 25V RADIAL</t>
-  </si>
-  <si>
-    <t>C2, C3</t>
-  </si>
-  <si>
-    <t>KEMET, Panasonic Electronic Components</t>
-  </si>
-  <si>
-    <t>ESK476M025AC3FA, ECA-1EM100B</t>
-  </si>
-  <si>
-    <t>399-ESK476M025AC3FACT-ND, P19522CT-ND</t>
+    <t>CL10B102KB8NNNC</t>
+  </si>
+  <si>
+    <t>CAP ALUM 47UF 20% 25V RADIAL</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>ESK476M025AC3FA</t>
+  </si>
+  <si>
+    <t>CAP ALUM 10UF 20% 25V RADIAL</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Panasonic Electronic Components</t>
+  </si>
+  <si>
+    <t>ECA-1EM100B</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 25V X5R 0603</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>CL10A104KA8NNNC</t>
   </si>
   <si>
     <t>DIODE SCHOTTKY 45V 50A D2PAK</t>
@@ -105,9 +111,6 @@
     <t>STPS5045SG-TR</t>
   </si>
   <si>
-    <t>497-13279-1-ND</t>
-  </si>
-  <si>
     <t>TERM BLOCK HDR 2POS VERT 5.08MM</t>
   </si>
   <si>
@@ -120,9 +123,6 @@
     <t>691311500002</t>
   </si>
   <si>
-    <t>732-2052-ND</t>
-  </si>
-  <si>
     <t>TERM BLOCK HDR 3POS VERT 5.08MM</t>
   </si>
   <si>
@@ -132,9 +132,6 @@
     <t>691311500103</t>
   </si>
   <si>
-    <t>732-2059-ND</t>
-  </si>
-  <si>
     <t>NUCLEO-32 STM32L432KC EVAL BRD</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>NUCLEO-L432KC</t>
   </si>
   <si>
-    <t>497-16592-ND</t>
-  </si>
-  <si>
     <t>TERM BLOCK HDR 4POS VERT 5.08MM</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>691311500104</t>
   </si>
   <si>
-    <t>732-2060-ND</t>
-  </si>
-  <si>
     <t>TERM BLOCK HDR 8POS VERT 5.08MM</t>
   </si>
   <si>
@@ -168,9 +159,6 @@
     <t>691311500108</t>
   </si>
   <si>
-    <t>732-2063-ND</t>
-  </si>
-  <si>
     <t>FIXED IND 10UH 9A 22 MOHM SMD</t>
   </si>
   <si>
@@ -183,37 +171,70 @@
     <t>125CDMCCDS-100MC</t>
   </si>
   <si>
-    <t>308-2561-1-ND</t>
-  </si>
-  <si>
     <t>MOSFET P-CH 40V 12A TO252</t>
   </si>
   <si>
     <t>Q1</t>
   </si>
   <si>
+    <t>Alpha &amp; Omega Semiconductor Inc.</t>
+  </si>
+  <si>
+    <t>AOD413A</t>
+  </si>
+  <si>
     <t>MOSFET N-CH 30V 6.9A/35A DPAK</t>
   </si>
   <si>
     <t>Q2_LSS3, Q2_LSS11, Q2_LSS12, Q2_LSS21, Q2_LSS22, Q3</t>
   </si>
   <si>
-    <t>[NoValue], RES 0 OHM JUMPER 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R4, R5, R6, R7_LSS3, R7_LSS11, R7_LSS12, R7_LSS21, R7_LSS22, R8_HSS1, R8_HSS2</t>
-  </si>
-  <si>
-    <t>[NoParam], Stackpole Electronics Inc</t>
-  </si>
-  <si>
-    <t>[NoParam], RMCF0603ZT0R00</t>
-  </si>
-  <si>
-    <t>[NoParam], Digi-Key</t>
-  </si>
-  <si>
-    <t>[NoParam], RMCF0603ZT0R00TR-ND</t>
+    <t>onsemi</t>
+  </si>
+  <si>
+    <t>NTD4815NHT4G</t>
+  </si>
+  <si>
+    <t>RES 82K OHM 5% 0603</t>
+  </si>
+  <si>
+    <t>R1, R4, R7_LSS3, R7_LSS11, R7_LSS12, R7_LSS21, R7_LSS22</t>
+  </si>
+  <si>
+    <t>RES 10 OHM 5% 0603</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>RES 0 OHM JUMPER 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics Inc</t>
+  </si>
+  <si>
+    <t>RMCF0603ZT0R00</t>
+  </si>
+  <si>
+    <t>RES 2.7K OHM 5% 0603</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>RES 20K OHM 5% 0603</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>RES 100 OHM 5% 0603</t>
+  </si>
+  <si>
+    <t>R8_HSS1, R8_HSS2</t>
   </si>
   <si>
     <t>PWM/VFM STEP-DOWN DCDC CONTROLLE</t>
@@ -228,13 +249,16 @@
     <t>R1224N102M-TR-FE</t>
   </si>
   <si>
-    <t>2129-R1224N102M-TR-FECT-ND</t>
-  </si>
-  <si>
     <t>SSR RELAY SPST-NO 2A 0-40V</t>
   </si>
   <si>
     <t>U2_HSS1, U2_HSS2</t>
+  </si>
+  <si>
+    <t>Toshiba Semiconductor and Storage</t>
+  </si>
+  <si>
+    <t>TLP241AF(TP4,F</t>
   </si>
 </sst>
 </file>
@@ -610,18 +634,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACFADB93-59CF-44CF-B9F2-A0F628D51832}">
-  <dimension ref="A1:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E01ED2E-19D7-49F1-B317-3B49A907BC8C}">
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="7" width="16.5703125" customWidth="1"/>
+    <col min="4" max="5" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -637,316 +661,343 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="D10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="1">
         <v>6</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="2" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="1">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="1">
-        <v>13</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C15" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>